<commit_message>
Tinggal buat change password
</commit_message>
<xml_diff>
--- a/Logika Tabel Guru dan Siswa.xlsx
+++ b/Logika Tabel Guru dan Siswa.xlsx
@@ -36,13 +36,13 @@
     <t>Tabel _Guru</t>
   </si>
   <si>
-    <t>Pelajaran_id</t>
-  </si>
-  <si>
     <t>Perkalian</t>
   </si>
   <si>
     <t>Group_Class</t>
+  </si>
+  <si>
+    <t>jurusan_id</t>
   </si>
 </sst>
 </file>
@@ -199,12 +199,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -213,6 +207,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,22 +527,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="K1" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="K1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
     </row>
     <row r="2" spans="4:16" x14ac:dyDescent="0.25">
       <c r="D2" s="3" t="s">
@@ -565,10 +565,10 @@
         <v>0</v>
       </c>
       <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="N2" s="6"/>
       <c r="O2" s="3" t="s">
@@ -579,34 +579,34 @@
       </c>
     </row>
     <row r="3" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D3" s="13">
-        <v>1</v>
-      </c>
-      <c r="E3" s="13">
+      <c r="D3" s="11">
+        <v>1</v>
+      </c>
+      <c r="E3" s="11">
         <v>1</v>
       </c>
       <c r="F3" s="1">
         <v>3</v>
       </c>
       <c r="G3" s="2"/>
-      <c r="H3" s="12">
+      <c r="H3" s="10">
         <f>D3+(E3*F3)</f>
         <v>4</v>
       </c>
       <c r="I3" s="1">
         <v>1</v>
       </c>
-      <c r="K3" s="14">
-        <v>1</v>
-      </c>
-      <c r="L3" s="14">
+      <c r="K3" s="12">
+        <v>1</v>
+      </c>
+      <c r="L3" s="12">
         <v>1</v>
       </c>
       <c r="M3" s="7">
         <v>3</v>
       </c>
       <c r="N3" s="8"/>
-      <c r="O3" s="15">
+      <c r="O3" s="13">
         <f>K3+(L3*M3)</f>
         <v>4</v>
       </c>
@@ -615,34 +615,34 @@
       </c>
     </row>
     <row r="4" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D4" s="13">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13">
+      <c r="D4" s="11">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11">
         <v>2</v>
       </c>
       <c r="F4" s="1">
         <v>3</v>
       </c>
       <c r="G4" s="2"/>
-      <c r="H4" s="12">
+      <c r="H4" s="10">
         <f t="shared" ref="H4:H20" si="0">D4+(E4*F4)</f>
         <v>7</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
       </c>
-      <c r="K4" s="14">
-        <v>1</v>
-      </c>
-      <c r="L4" s="14">
+      <c r="K4" s="12">
+        <v>1</v>
+      </c>
+      <c r="L4" s="12">
         <v>2</v>
       </c>
       <c r="M4" s="7">
         <v>3</v>
       </c>
       <c r="N4" s="8"/>
-      <c r="O4" s="15">
+      <c r="O4" s="13">
         <f t="shared" ref="O4:O8" si="1">K4+(L4*M4)</f>
         <v>7</v>
       </c>
@@ -651,34 +651,34 @@
       </c>
     </row>
     <row r="5" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D5" s="13">
-        <v>1</v>
-      </c>
-      <c r="E5" s="13">
+      <c r="D5" s="11">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11">
         <v>3</v>
       </c>
       <c r="F5" s="1">
         <v>3</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="12">
+      <c r="H5" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="I5" s="1">
         <v>3</v>
       </c>
-      <c r="K5" s="14">
-        <v>2</v>
-      </c>
-      <c r="L5" s="14">
+      <c r="K5" s="12">
+        <v>2</v>
+      </c>
+      <c r="L5" s="12">
         <v>1</v>
       </c>
       <c r="M5" s="7">
         <v>3</v>
       </c>
       <c r="N5" s="8"/>
-      <c r="O5" s="15">
+      <c r="O5" s="13">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -687,34 +687,34 @@
       </c>
     </row>
     <row r="6" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D6" s="13">
-        <v>2</v>
-      </c>
-      <c r="E6" s="13">
+      <c r="D6" s="11">
+        <v>2</v>
+      </c>
+      <c r="E6" s="11">
         <v>1</v>
       </c>
       <c r="F6" s="1">
         <v>3</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="12">
+      <c r="H6" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I6" s="1">
         <v>4</v>
       </c>
-      <c r="K6" s="14">
-        <v>2</v>
-      </c>
-      <c r="L6" s="14">
+      <c r="K6" s="12">
+        <v>2</v>
+      </c>
+      <c r="L6" s="12">
         <v>2</v>
       </c>
       <c r="M6" s="7">
         <v>3</v>
       </c>
       <c r="N6" s="8"/>
-      <c r="O6" s="15">
+      <c r="O6" s="13">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
@@ -723,34 +723,34 @@
       </c>
     </row>
     <row r="7" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D7" s="13">
-        <v>2</v>
-      </c>
-      <c r="E7" s="13">
+      <c r="D7" s="11">
+        <v>2</v>
+      </c>
+      <c r="E7" s="11">
         <v>2</v>
       </c>
       <c r="F7" s="1">
         <v>3</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="12">
+      <c r="H7" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="I7" s="1">
         <v>5</v>
       </c>
-      <c r="K7" s="14">
-        <v>3</v>
-      </c>
-      <c r="L7" s="14">
+      <c r="K7" s="12">
+        <v>3</v>
+      </c>
+      <c r="L7" s="12">
         <v>1</v>
       </c>
       <c r="M7" s="7">
         <v>3</v>
       </c>
       <c r="N7" s="8"/>
-      <c r="O7" s="15">
+      <c r="O7" s="13">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
@@ -759,34 +759,34 @@
       </c>
     </row>
     <row r="8" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D8" s="13">
-        <v>2</v>
-      </c>
-      <c r="E8" s="13">
+      <c r="D8" s="11">
+        <v>2</v>
+      </c>
+      <c r="E8" s="11">
         <v>3</v>
       </c>
       <c r="F8" s="1">
         <v>3</v>
       </c>
       <c r="G8" s="2"/>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="I8" s="1">
         <v>6</v>
       </c>
-      <c r="K8" s="14">
-        <v>3</v>
-      </c>
-      <c r="L8" s="14">
+      <c r="K8" s="12">
+        <v>3</v>
+      </c>
+      <c r="L8" s="12">
         <v>2</v>
       </c>
       <c r="M8" s="7">
         <v>3</v>
       </c>
       <c r="N8" s="9"/>
-      <c r="O8" s="15">
+      <c r="O8" s="13">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
@@ -795,17 +795,17 @@
       </c>
     </row>
     <row r="9" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D9" s="13">
-        <v>3</v>
-      </c>
-      <c r="E9" s="13">
+      <c r="D9" s="11">
+        <v>3</v>
+      </c>
+      <c r="E9" s="11">
         <v>1</v>
       </c>
       <c r="F9" s="1">
         <v>3</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="12">
+      <c r="H9" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -814,17 +814,17 @@
       </c>
     </row>
     <row r="10" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D10" s="13">
-        <v>3</v>
-      </c>
-      <c r="E10" s="13">
+      <c r="D10" s="11">
+        <v>3</v>
+      </c>
+      <c r="E10" s="11">
         <v>2</v>
       </c>
       <c r="F10" s="1">
         <v>3</v>
       </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="12">
+      <c r="H10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -833,17 +833,17 @@
       </c>
     </row>
     <row r="11" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D11" s="13">
-        <v>3</v>
-      </c>
-      <c r="E11" s="13">
+      <c r="D11" s="11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="11">
         <v>3</v>
       </c>
       <c r="F11" s="1">
         <v>3</v>
       </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="12">
+      <c r="H11" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -852,17 +852,17 @@
       </c>
     </row>
     <row r="12" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D12" s="13">
-        <v>1</v>
-      </c>
-      <c r="E12" s="13">
+      <c r="D12" s="11">
+        <v>1</v>
+      </c>
+      <c r="E12" s="11">
         <v>4</v>
       </c>
       <c r="F12" s="1">
         <v>3</v>
       </c>
       <c r="G12" s="2"/>
-      <c r="H12" s="12">
+      <c r="H12" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -871,17 +871,17 @@
       </c>
     </row>
     <row r="13" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D13" s="13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13">
+      <c r="D13" s="11">
+        <v>1</v>
+      </c>
+      <c r="E13" s="11">
         <v>5</v>
       </c>
       <c r="F13" s="1">
         <v>3</v>
       </c>
       <c r="G13" s="2"/>
-      <c r="H13" s="12">
+      <c r="H13" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -890,17 +890,17 @@
       </c>
     </row>
     <row r="14" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D14" s="13">
-        <v>1</v>
-      </c>
-      <c r="E14" s="13">
+      <c r="D14" s="11">
+        <v>1</v>
+      </c>
+      <c r="E14" s="11">
         <v>6</v>
       </c>
       <c r="F14" s="1">
         <v>3</v>
       </c>
       <c r="G14" s="2"/>
-      <c r="H14" s="12">
+      <c r="H14" s="10">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
@@ -909,17 +909,17 @@
       </c>
     </row>
     <row r="15" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D15" s="13">
-        <v>2</v>
-      </c>
-      <c r="E15" s="13">
+      <c r="D15" s="11">
+        <v>2</v>
+      </c>
+      <c r="E15" s="11">
         <v>4</v>
       </c>
       <c r="F15" s="1">
         <v>3</v>
       </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="12">
+      <c r="H15" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -928,17 +928,17 @@
       </c>
     </row>
     <row r="16" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D16" s="13">
-        <v>2</v>
-      </c>
-      <c r="E16" s="13">
+      <c r="D16" s="11">
+        <v>2</v>
+      </c>
+      <c r="E16" s="11">
         <v>5</v>
       </c>
       <c r="F16" s="1">
         <v>3</v>
       </c>
       <c r="G16" s="2"/>
-      <c r="H16" s="12">
+      <c r="H16" s="10">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
@@ -947,17 +947,17 @@
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D17" s="13">
-        <v>2</v>
-      </c>
-      <c r="E17" s="13">
+      <c r="D17" s="11">
+        <v>2</v>
+      </c>
+      <c r="E17" s="11">
         <v>6</v>
       </c>
       <c r="F17" s="1">
         <v>3</v>
       </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="12">
+      <c r="H17" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
@@ -966,17 +966,17 @@
       </c>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D18" s="13">
-        <v>3</v>
-      </c>
-      <c r="E18" s="13">
+      <c r="D18" s="11">
+        <v>3</v>
+      </c>
+      <c r="E18" s="11">
         <v>4</v>
       </c>
       <c r="F18" s="1">
         <v>3</v>
       </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="12">
+      <c r="H18" s="10">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -985,17 +985,17 @@
       </c>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="13">
-        <v>3</v>
-      </c>
-      <c r="E19" s="13">
+      <c r="D19" s="11">
+        <v>3</v>
+      </c>
+      <c r="E19" s="11">
         <v>5</v>
       </c>
       <c r="F19" s="1">
         <v>3</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="12">
+      <c r="H19" s="10">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
@@ -1004,17 +1004,17 @@
       </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="13">
-        <v>3</v>
-      </c>
-      <c r="E20" s="13">
+      <c r="D20" s="11">
+        <v>3</v>
+      </c>
+      <c r="E20" s="11">
         <v>6</v>
       </c>
       <c r="F20" s="1">
         <v>3</v>
       </c>
       <c r="G20" s="4"/>
-      <c r="H20" s="12">
+      <c r="H20" s="10">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>

</xml_diff>